<commit_message>
Modification tot he fishing method SDMX model
</commit_message>
<xml_diff>
--- a/model/Fishing_method_SDMX_Model.xlsx
+++ b/model/Fishing_method_SDMX_Model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\rara\RAP\Agriculture\sdd-household-primary-activity-processing\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4389069D-66AA-49B4-9785-FD4FC58F23AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F7ABFA9-496B-4CBA-8E09-FA83CE5236CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="135" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DSD" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="64">
   <si>
     <t>Concepts</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Indicator</t>
   </si>
   <si>
-    <t>CL_INDICATOR</t>
-  </si>
-  <si>
     <t>OBS_VALUE</t>
   </si>
   <si>
@@ -227,25 +224,16 @@
     <t>Othe fishing method</t>
   </si>
   <si>
-    <t>CL_FISHING_SPEAR</t>
-  </si>
-  <si>
-    <t>CL_FISHING_GLEANING</t>
-  </si>
-  <si>
-    <t>CL_FISHING_LINE</t>
-  </si>
-  <si>
-    <t>CL_FISHING_NET</t>
-  </si>
-  <si>
-    <t>CL_FISHING_OTHER_METHOD</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>CL_FISHING_METHOD_INDICATORS</t>
+  </si>
+  <si>
+    <t>CL_COM_YESNO</t>
   </si>
 </sst>
 </file>
@@ -602,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +601,7 @@
     <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -725,18 +713,18 @@
         <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
         <v>44</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
       </c>
       <c r="C6" t="s">
         <v>9</v>
@@ -748,7 +736,7 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G6" t="s">
         <v>9</v>
@@ -756,10 +744,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>48</v>
       </c>
       <c r="C7" t="s">
         <v>9</v>
@@ -771,7 +759,7 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G7" t="s">
         <v>9</v>
@@ -779,13 +767,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" t="s">
         <v>10</v>
@@ -794,21 +782,21 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G8" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
         <v>52</v>
       </c>
-      <c r="B9" t="s">
-        <v>53</v>
-      </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
         <v>10</v>
@@ -820,18 +808,18 @@
         <v>63</v>
       </c>
       <c r="G9" t="s">
-        <v>38</v>
+        <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
         <v>55</v>
       </c>
-      <c r="B10" t="s">
-        <v>56</v>
-      </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
@@ -840,18 +828,21 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" t="s">
         <v>57</v>
       </c>
-      <c r="B11" t="s">
-        <v>58</v>
-      </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
         <v>10</v>
@@ -860,18 +851,21 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>61</v>
+        <v>63</v>
+      </c>
+      <c r="G11" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
         <v>59</v>
       </c>
-      <c r="B12" t="s">
-        <v>60</v>
-      </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
         <v>10</v>
@@ -880,27 +874,30 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="G12" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
         <v>25</v>
-      </c>
-      <c r="C13" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
-        <v>26</v>
       </c>
       <c r="E13" t="s">
         <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G13" t="s">
         <v>17</v>
@@ -908,22 +905,22 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>28</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
         <v>29</v>
-      </c>
-      <c r="C14" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
         <v>9</v>
@@ -931,22 +928,22 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
       </c>
       <c r="F15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G15" t="s">
         <v>9</v>
@@ -954,22 +951,22 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="B16" t="s">
-        <v>34</v>
-      </c>
       <c r="C16" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G16" t="s">
         <v>9</v>
@@ -985,7 +982,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14318586-0638-4AAA-9EF3-71D17652D048}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -996,7 +993,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1004,23 +1001,23 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1043,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1051,23 +1048,23 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1090,7 +1087,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1098,23 +1095,23 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1137,7 +1134,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1145,23 +1142,23 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -1189,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1197,23 +1194,23 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1263,23 +1260,23 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>